<commit_message>
se agregaron las barras de progreso
</commit_message>
<xml_diff>
--- a/NRFM_Auditoria/NRFM_Auditoria/bin/Debug/net8.0-windows/Extracciones/Responsables/5-2024/ALFREDO JIMENEZ.xlsx
+++ b/NRFM_Auditoria/NRFM_Auditoria/bin/Debug/net8.0-windows/Extracciones/Responsables/5-2024/ALFREDO JIMENEZ.xlsx
@@ -10,20 +10,18 @@
     <x:sheet name="EKIP" sheetId="3" r:id="rId3"/>
     <x:sheet name="EKIPINTER" sheetId="4" r:id="rId4"/>
     <x:sheet name="IAPI" sheetId="5" r:id="rId5"/>
-    <x:sheet name="PROCOTIZA" sheetId="6" r:id="rId6"/>
-    <x:sheet name="PRODESK" sheetId="7" r:id="rId7"/>
-    <x:sheet name="DECISION ENGINE" sheetId="8" r:id="rId8"/>
-    <x:sheet name="WEBAPP" sheetId="9" r:id="rId9"/>
+    <x:sheet name="PRODESK" sheetId="6" r:id="rId6"/>
+    <x:sheet name="DECISION ENGINE" sheetId="7" r:id="rId7"/>
+    <x:sheet name="WEBAPP" sheetId="8" r:id="rId8"/>
   </x:sheets>
   <x:definedNames>
     <x:definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CSYSO!$A$5:$L$5</x:definedName>
     <x:definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EKIP!$A$5:$I$5</x:definedName>
     <x:definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EKIPINTER!$A$5:$H$5</x:definedName>
     <x:definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">IAPI!$A$5:$I$5</x:definedName>
-    <x:definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">PROCOTIZA!$A$5:$K$5</x:definedName>
-    <x:definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">PRODESK!$A$5:$K$5</x:definedName>
-    <x:definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'DECISION ENGINE'!$A$5:$J$5</x:definedName>
-    <x:definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">WEBAPP!$A$5:$K$5</x:definedName>
+    <x:definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">PRODESK!$A$5:$K$5</x:definedName>
+    <x:definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'DECISION ENGINE'!$A$5:$J$5</x:definedName>
+    <x:definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">WEBAPP!$A$5:$K$5</x:definedName>
   </x:definedNames>
   <x:calcPr calcId="125725"/>
 </x:workbook>
@@ -3066,43 +3064,13 @@
     <x:t>JOSELYNE BERNAL AGUADO</x:t>
   </x:si>
   <x:si>
-    <x:t>PROCOTIZA</x:t>
+    <x:t>PRODESK</x:t>
   </x:si>
   <x:si>
     <x:t>Fecha de Creacion</x:t>
   </x:si>
   <x:si>
     <x:t>Ultimo Acceso</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CALIDAD</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Joselyne Guadalupe Bernal Aguado</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CALJBA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Raúl Capetillo Cervantes</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CALRCC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Miguel Angel Gallegos Gutierrez</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CALMGG</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sergio Ricardo Romero Gonzalez</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CALSRM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PRODESK</x:t>
   </x:si>
   <x:si>
     <x:t>ANTONY JR CORNELIO PEÑA</x:t>
@@ -17044,259 +17012,6 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:J11"/>
-  <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:cols>
-    <x:col min="1" max="1" width="11.282054" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="33.853482" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="10.139196" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="40.424911" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="8.710625" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="19.282054" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="15.853482" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="17.567768" style="0" customWidth="1"/>
-    <x:col min="9" max="9" width="18.567768" style="0" customWidth="1"/>
-    <x:col min="10" max="10" width="14.853482" style="0" customWidth="1"/>
-  </x:cols>
-  <x:sheetData>
-    <x:row r="1" spans="1:10">
-      <x:c r="D1" s="1" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:10">
-      <x:c r="D2" s="1" t="s">
-        <x:v>1011</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:10">
-      <x:c r="D3" s="1" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:10">
-      <x:c r="D4" s="1" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:10">
-      <x:c r="A5" s="2" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B5" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="C5" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D5" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E5" s="2" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="F5" s="2" t="s">
-        <x:v>1012</x:v>
-      </x:c>
-      <x:c r="G5" s="2" t="s">
-        <x:v>1013</x:v>
-      </x:c>
-      <x:c r="H5" s="2" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="I5" s="2" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="J5" s="2" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:10">
-      <x:c r="A6" s="3" t="s">
-        <x:v>1011</x:v>
-      </x:c>
-      <x:c r="B6" s="3" t="s">
-        <x:v>889</x:v>
-      </x:c>
-      <x:c r="C6" s="3" t="s">
-        <x:v>490</x:v>
-      </x:c>
-      <x:c r="D6" s="3" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E6" s="3" t="s">
-        <x:v>1014</x:v>
-      </x:c>
-      <x:c r="F6" s="4">
-        <x:v>45237</x:v>
-      </x:c>
-      <x:c r="G6" s="4">
-        <x:v>45334</x:v>
-      </x:c>
-      <x:c r="H6" s="3" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="I6" s="3"/>
-      <x:c r="J6" s="3"/>
-    </x:row>
-    <x:row r="7" spans="1:10">
-      <x:c r="A7" s="3" t="s">
-        <x:v>1011</x:v>
-      </x:c>
-      <x:c r="B7" s="3" t="s">
-        <x:v>732</x:v>
-      </x:c>
-      <x:c r="C7" s="3" t="s">
-        <x:v>641</x:v>
-      </x:c>
-      <x:c r="D7" s="3" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E7" s="3" t="s">
-        <x:v>1014</x:v>
-      </x:c>
-      <x:c r="F7" s="4">
-        <x:v>45180</x:v>
-      </x:c>
-      <x:c r="G7" s="4">
-        <x:v>45355</x:v>
-      </x:c>
-      <x:c r="H7" s="3" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="I7" s="3"/>
-      <x:c r="J7" s="3"/>
-    </x:row>
-    <x:row r="8" spans="1:10">
-      <x:c r="A8" s="3" t="s">
-        <x:v>1011</x:v>
-      </x:c>
-      <x:c r="B8" s="3" t="s">
-        <x:v>1015</x:v>
-      </x:c>
-      <x:c r="C8" s="3" t="s">
-        <x:v>1016</x:v>
-      </x:c>
-      <x:c r="D8" s="3" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E8" s="3" t="s">
-        <x:v>1014</x:v>
-      </x:c>
-      <x:c r="F8" s="4">
-        <x:v>44757</x:v>
-      </x:c>
-      <x:c r="G8" s="4">
-        <x:v>45355</x:v>
-      </x:c>
-      <x:c r="H8" s="3" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="I8" s="3"/>
-      <x:c r="J8" s="3"/>
-    </x:row>
-    <x:row r="9" spans="1:10">
-      <x:c r="A9" s="3" t="s">
-        <x:v>1011</x:v>
-      </x:c>
-      <x:c r="B9" s="3" t="s">
-        <x:v>1017</x:v>
-      </x:c>
-      <x:c r="C9" s="3" t="s">
-        <x:v>1018</x:v>
-      </x:c>
-      <x:c r="D9" s="3" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E9" s="3" t="s">
-        <x:v>1014</x:v>
-      </x:c>
-      <x:c r="F9" s="4">
-        <x:v>44757</x:v>
-      </x:c>
-      <x:c r="G9" s="4">
-        <x:v>45355</x:v>
-      </x:c>
-      <x:c r="H9" s="3" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="I9" s="3"/>
-      <x:c r="J9" s="3"/>
-    </x:row>
-    <x:row r="10" spans="1:10">
-      <x:c r="A10" s="3" t="s">
-        <x:v>1011</x:v>
-      </x:c>
-      <x:c r="B10" s="3" t="s">
-        <x:v>1019</x:v>
-      </x:c>
-      <x:c r="C10" s="3" t="s">
-        <x:v>1020</x:v>
-      </x:c>
-      <x:c r="D10" s="3" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E10" s="3" t="s">
-        <x:v>1014</x:v>
-      </x:c>
-      <x:c r="F10" s="4">
-        <x:v>44757</x:v>
-      </x:c>
-      <x:c r="G10" s="4">
-        <x:v>45355</x:v>
-      </x:c>
-      <x:c r="H10" s="3" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="I10" s="3"/>
-      <x:c r="J10" s="3"/>
-    </x:row>
-    <x:row r="11" spans="1:10">
-      <x:c r="A11" s="3" t="s">
-        <x:v>1011</x:v>
-      </x:c>
-      <x:c r="B11" s="3" t="s">
-        <x:v>1021</x:v>
-      </x:c>
-      <x:c r="C11" s="3" t="s">
-        <x:v>1022</x:v>
-      </x:c>
-      <x:c r="D11" s="3" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E11" s="3" t="s">
-        <x:v>1014</x:v>
-      </x:c>
-      <x:c r="F11" s="4">
-        <x:v>44757</x:v>
-      </x:c>
-      <x:c r="G11" s="4">
-        <x:v>45355</x:v>
-      </x:c>
-      <x:c r="H11" s="3" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="I11" s="3"/>
-      <x:c r="J11" s="3"/>
-    </x:row>
-  </x:sheetData>
-  <x:autoFilter ref="A5:K5"/>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
   <x:dimension ref="A1:J14"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
@@ -17322,7 +17037,7 @@
     </x:row>
     <x:row r="2" spans="1:10">
       <x:c r="D2" s="1" t="s">
-        <x:v>1023</x:v>
+        <x:v>1011</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:10">
@@ -17369,19 +17084,19 @@
     </x:row>
     <x:row r="6" spans="1:10">
       <x:c r="A6" s="3" t="s">
-        <x:v>1023</x:v>
+        <x:v>1011</x:v>
       </x:c>
       <x:c r="B6" s="3" t="s">
-        <x:v>1024</x:v>
+        <x:v>1014</x:v>
       </x:c>
       <x:c r="C6" s="3" t="s">
         <x:v>382</x:v>
       </x:c>
       <x:c r="D6" s="3" t="s">
-        <x:v>1025</x:v>
+        <x:v>1015</x:v>
       </x:c>
       <x:c r="E6" s="3" t="s">
-        <x:v>1026</x:v>
+        <x:v>1016</x:v>
       </x:c>
       <x:c r="F6" s="4">
         <x:v>45161</x:v>
@@ -17397,19 +17112,19 @@
     </x:row>
     <x:row r="7" spans="1:10">
       <x:c r="A7" s="3" t="s">
-        <x:v>1023</x:v>
+        <x:v>1011</x:v>
       </x:c>
       <x:c r="B7" s="3" t="s">
-        <x:v>1027</x:v>
+        <x:v>1017</x:v>
       </x:c>
       <x:c r="C7" s="3" t="s">
         <x:v>765</x:v>
       </x:c>
       <x:c r="D7" s="3" t="s">
-        <x:v>1025</x:v>
+        <x:v>1015</x:v>
       </x:c>
       <x:c r="E7" s="3" t="s">
-        <x:v>1028</x:v>
+        <x:v>1018</x:v>
       </x:c>
       <x:c r="F7" s="4">
         <x:v>45098</x:v>
@@ -17425,19 +17140,19 @@
     </x:row>
     <x:row r="8" spans="1:10">
       <x:c r="A8" s="3" t="s">
-        <x:v>1023</x:v>
+        <x:v>1011</x:v>
       </x:c>
       <x:c r="B8" s="3" t="s">
-        <x:v>1029</x:v>
+        <x:v>1019</x:v>
       </x:c>
       <x:c r="C8" s="3" t="s">
         <x:v>734</x:v>
       </x:c>
       <x:c r="D8" s="3" t="s">
-        <x:v>1025</x:v>
+        <x:v>1015</x:v>
       </x:c>
       <x:c r="E8" s="3" t="s">
-        <x:v>1028</x:v>
+        <x:v>1018</x:v>
       </x:c>
       <x:c r="F8" s="4">
         <x:v>45098</x:v>
@@ -17453,19 +17168,19 @@
     </x:row>
     <x:row r="9" spans="1:10">
       <x:c r="A9" s="3" t="s">
-        <x:v>1023</x:v>
+        <x:v>1011</x:v>
       </x:c>
       <x:c r="B9" s="3" t="s">
-        <x:v>1030</x:v>
+        <x:v>1020</x:v>
       </x:c>
       <x:c r="C9" s="3" t="s">
         <x:v>487</x:v>
       </x:c>
       <x:c r="D9" s="3" t="s">
-        <x:v>1025</x:v>
+        <x:v>1015</x:v>
       </x:c>
       <x:c r="E9" s="3" t="s">
-        <x:v>1031</x:v>
+        <x:v>1021</x:v>
       </x:c>
       <x:c r="F9" s="4">
         <x:v>45202</x:v>
@@ -17481,19 +17196,19 @@
     </x:row>
     <x:row r="10" spans="1:10">
       <x:c r="A10" s="3" t="s">
+        <x:v>1011</x:v>
+      </x:c>
+      <x:c r="B10" s="3" t="s">
+        <x:v>1022</x:v>
+      </x:c>
+      <x:c r="C10" s="3" t="s">
         <x:v>1023</x:v>
       </x:c>
-      <x:c r="B10" s="3" t="s">
-        <x:v>1032</x:v>
-      </x:c>
-      <x:c r="C10" s="3" t="s">
-        <x:v>1033</x:v>
-      </x:c>
       <x:c r="D10" s="3" t="s">
-        <x:v>1025</x:v>
+        <x:v>1015</x:v>
       </x:c>
       <x:c r="E10" s="3" t="s">
-        <x:v>1034</x:v>
+        <x:v>1024</x:v>
       </x:c>
       <x:c r="F10" s="4">
         <x:v>45156</x:v>
@@ -17509,19 +17224,19 @@
     </x:row>
     <x:row r="11" spans="1:10">
       <x:c r="A11" s="3" t="s">
-        <x:v>1023</x:v>
+        <x:v>1011</x:v>
       </x:c>
       <x:c r="B11" s="3" t="s">
-        <x:v>1035</x:v>
+        <x:v>1025</x:v>
       </x:c>
       <x:c r="C11" s="3" t="s">
         <x:v>300</x:v>
       </x:c>
       <x:c r="D11" s="3" t="s">
-        <x:v>1025</x:v>
+        <x:v>1015</x:v>
       </x:c>
       <x:c r="E11" s="3" t="s">
-        <x:v>1026</x:v>
+        <x:v>1016</x:v>
       </x:c>
       <x:c r="F11" s="4">
         <x:v>45212</x:v>
@@ -17537,19 +17252,19 @@
     </x:row>
     <x:row r="12" spans="1:10">
       <x:c r="A12" s="3" t="s">
-        <x:v>1023</x:v>
+        <x:v>1011</x:v>
       </x:c>
       <x:c r="B12" s="3" t="s">
-        <x:v>1036</x:v>
+        <x:v>1026</x:v>
       </x:c>
       <x:c r="C12" s="3" t="s">
         <x:v>133</x:v>
       </x:c>
       <x:c r="D12" s="3" t="s">
-        <x:v>1025</x:v>
+        <x:v>1015</x:v>
       </x:c>
       <x:c r="E12" s="3" t="s">
-        <x:v>1026</x:v>
+        <x:v>1016</x:v>
       </x:c>
       <x:c r="F12" s="4">
         <x:v>45296</x:v>
@@ -17565,7 +17280,7 @@
     </x:row>
     <x:row r="13" spans="1:10">
       <x:c r="A13" s="3" t="s">
-        <x:v>1023</x:v>
+        <x:v>1011</x:v>
       </x:c>
       <x:c r="B13" s="3" t="s">
         <x:v>968</x:v>
@@ -17574,10 +17289,10 @@
         <x:v>539</x:v>
       </x:c>
       <x:c r="D13" s="3" t="s">
-        <x:v>1025</x:v>
+        <x:v>1015</x:v>
       </x:c>
       <x:c r="E13" s="3" t="s">
-        <x:v>1026</x:v>
+        <x:v>1016</x:v>
       </x:c>
       <x:c r="F13" s="4">
         <x:v>45161</x:v>
@@ -17593,25 +17308,25 @@
     </x:row>
     <x:row r="14" spans="1:10">
       <x:c r="A14" s="3" t="s">
-        <x:v>1023</x:v>
+        <x:v>1011</x:v>
       </x:c>
       <x:c r="B14" s="3" t="s">
-        <x:v>1037</x:v>
+        <x:v>1027</x:v>
       </x:c>
       <x:c r="C14" s="3" t="s">
-        <x:v>1038</x:v>
+        <x:v>1028</x:v>
       </x:c>
       <x:c r="D14" s="3" t="s">
-        <x:v>1025</x:v>
+        <x:v>1015</x:v>
       </x:c>
       <x:c r="E14" s="3" t="s">
-        <x:v>1026</x:v>
+        <x:v>1016</x:v>
       </x:c>
       <x:c r="F14" s="4">
         <x:v>45330</x:v>
       </x:c>
       <x:c r="G14" s="3" t="s">
-        <x:v>1039</x:v>
+        <x:v>1029</x:v>
       </x:c>
       <x:c r="H14" s="3" t="s">
         <x:v>20</x:v>
@@ -17629,7 +17344,7 @@
 </x:worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -17658,7 +17373,7 @@
     </x:row>
     <x:row r="2" spans="1:9">
       <x:c r="D2" s="1" t="s">
-        <x:v>1040</x:v>
+        <x:v>1030</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:9">
@@ -17679,7 +17394,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="C5" s="2" t="s">
-        <x:v>1041</x:v>
+        <x:v>1031</x:v>
       </x:c>
       <x:c r="D5" s="2" t="s">
         <x:v>7</x:v>
@@ -17702,19 +17417,19 @@
     </x:row>
     <x:row r="6" spans="1:9">
       <x:c r="A6" s="3" t="s">
-        <x:v>1042</x:v>
+        <x:v>1032</x:v>
       </x:c>
       <x:c r="B6" s="3" t="s">
-        <x:v>1043</x:v>
+        <x:v>1033</x:v>
       </x:c>
       <x:c r="C6" s="3" t="s">
-        <x:v>1044</x:v>
+        <x:v>1034</x:v>
       </x:c>
       <x:c r="D6" s="3" t="s">
-        <x:v>1045</x:v>
+        <x:v>1035</x:v>
       </x:c>
       <x:c r="E6" s="3" t="s">
-        <x:v>1046</x:v>
+        <x:v>1036</x:v>
       </x:c>
       <x:c r="F6" s="4">
         <x:v>44443</x:v>
@@ -17727,19 +17442,19 @@
     </x:row>
     <x:row r="7" spans="1:9">
       <x:c r="A7" s="3" t="s">
-        <x:v>1042</x:v>
+        <x:v>1032</x:v>
       </x:c>
       <x:c r="B7" s="3" t="s">
-        <x:v>1047</x:v>
+        <x:v>1037</x:v>
       </x:c>
       <x:c r="C7" s="3" t="s">
-        <x:v>1044</x:v>
+        <x:v>1034</x:v>
       </x:c>
       <x:c r="D7" s="3" t="s">
-        <x:v>1045</x:v>
+        <x:v>1035</x:v>
       </x:c>
       <x:c r="E7" s="3" t="s">
-        <x:v>1046</x:v>
+        <x:v>1036</x:v>
       </x:c>
       <x:c r="F7" s="4">
         <x:v>44874</x:v>
@@ -17752,19 +17467,19 @@
     </x:row>
     <x:row r="8" spans="1:9">
       <x:c r="A8" s="3" t="s">
-        <x:v>1042</x:v>
+        <x:v>1032</x:v>
       </x:c>
       <x:c r="B8" s="3" t="s">
-        <x:v>1048</x:v>
+        <x:v>1038</x:v>
       </x:c>
       <x:c r="C8" s="3" t="s">
-        <x:v>1044</x:v>
+        <x:v>1034</x:v>
       </x:c>
       <x:c r="D8" s="3" t="s">
-        <x:v>1045</x:v>
+        <x:v>1035</x:v>
       </x:c>
       <x:c r="E8" s="3" t="s">
-        <x:v>1046</x:v>
+        <x:v>1036</x:v>
       </x:c>
       <x:c r="F8" s="4">
         <x:v>44874</x:v>
@@ -17777,19 +17492,19 @@
     </x:row>
     <x:row r="9" spans="1:9">
       <x:c r="A9" s="3" t="s">
-        <x:v>1042</x:v>
+        <x:v>1032</x:v>
       </x:c>
       <x:c r="B9" s="3" t="s">
-        <x:v>1049</x:v>
+        <x:v>1039</x:v>
       </x:c>
       <x:c r="C9" s="3" t="s">
-        <x:v>1044</x:v>
+        <x:v>1034</x:v>
       </x:c>
       <x:c r="D9" s="3" t="s">
-        <x:v>1045</x:v>
+        <x:v>1035</x:v>
       </x:c>
       <x:c r="E9" s="3" t="s">
-        <x:v>1046</x:v>
+        <x:v>1036</x:v>
       </x:c>
       <x:c r="F9" s="4">
         <x:v>44443</x:v>
@@ -17810,7 +17525,7 @@
 </x:worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -17840,7 +17555,7 @@
     </x:row>
     <x:row r="2" spans="1:10">
       <x:c r="D2" s="1" t="s">
-        <x:v>1050</x:v>
+        <x:v>1040</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:10">
@@ -17867,13 +17582,13 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="E5" s="2" t="s">
-        <x:v>1051</x:v>
+        <x:v>1041</x:v>
       </x:c>
       <x:c r="F5" s="2" t="s">
         <x:v>1012</x:v>
       </x:c>
       <x:c r="G5" s="2" t="s">
-        <x:v>1052</x:v>
+        <x:v>1042</x:v>
       </x:c>
       <x:c r="H5" s="2" t="s">
         <x:v>12</x:v>
@@ -17887,19 +17602,19 @@
     </x:row>
     <x:row r="6" spans="1:10">
       <x:c r="A6" s="3" t="s">
-        <x:v>1050</x:v>
+        <x:v>1040</x:v>
       </x:c>
       <x:c r="B6" s="3" t="s">
-        <x:v>1053</x:v>
+        <x:v>1043</x:v>
       </x:c>
       <x:c r="C6" s="3" t="s">
         <x:v>782</x:v>
       </x:c>
       <x:c r="D6" s="3" t="s">
-        <x:v>1025</x:v>
+        <x:v>1015</x:v>
       </x:c>
       <x:c r="E6" s="3" t="s">
-        <x:v>1054</x:v>
+        <x:v>1044</x:v>
       </x:c>
       <x:c r="F6" s="4">
         <x:v>29804</x:v>

</xml_diff>